<commit_message>
tambah UAT polres pada word
</commit_message>
<xml_diff>
--- a/Rangkuman Jurnal.xlsx
+++ b/Rangkuman Jurnal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44520642-0E55-42DF-A21A-124C7E0D709B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12944E3-CBBC-44AB-83E0-20AE016C4871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Konteks atau tema jurnal</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>Tahun</t>
+  </si>
+  <si>
+    <t>Klaster Kosong</t>
+  </si>
+  <si>
+    <t>CLUSTERING LOYALITAS PELANGGAN DENGAN MODEL RFM (REFENCY, FREQUENCY, MONETARY) DAN METODE K-MEANS BERBASIS MEDIAN</t>
+  </si>
+  <si>
+    <t>Ahmad Supriadi 1 , Moh. Sukron 2 , Mochammad Faid 3</t>
+  </si>
+  <si>
+    <t>CORE AI</t>
+  </si>
+  <si>
+    <t>Tahun 2021</t>
   </si>
 </sst>
 </file>
@@ -112,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -126,13 +141,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -418,7 +439,7 @@
   <dimension ref="A2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +474,7 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -468,37 +489,49 @@
       <c r="E3" s="1">
         <v>5</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>44927</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>45231</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2 file word ada yang pake coding ada yang tanpa
</commit_message>
<xml_diff>
--- a/Rangkuman Jurnal.xlsx
+++ b/Rangkuman Jurnal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63975D60-F2D8-4F71-BDA5-B556EA89558F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AAF447-FBF1-427E-9BA4-3A08E7AEDA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,13 +438,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -453,20 +447,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -477,6 +459,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,31 +779,31 @@
       <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -815,17 +815,17 @@
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="3">
         <v>5</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>44927</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -835,19 +835,19 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="3">
         <v>3</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <v>45231</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -856,74 +856,74 @@
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="7">
         <v>44593</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -935,285 +935,285 @@
       <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="9">
         <v>45129</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="18">
         <v>3</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="17">
         <v>44587</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="13">
         <v>6</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="13">
         <v>2024</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="13">
         <v>7</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="13">
         <v>4</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="13">
         <v>2023</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="13">
         <v>8</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="14">
         <v>4</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="14">
         <v>2023</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="13">
         <v>9</v>
       </c>
       <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="14">
         <v>5</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="14">
         <v>2024</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="13">
         <v>10</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="13">
         <v>3</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="13">
         <v>2024</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -1222,7 +1222,7 @@
       <c r="B25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D25" t="s">
@@ -1271,13 +1271,13 @@
       <c r="B27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="10" t="s">
         <v>81</v>
       </c>
       <c r="F27" s="2">
@@ -1317,42 +1317,42 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="13">
         <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="13">
         <v>4</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="13">
         <v>2022</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -1413,27 +1413,27 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="I15:I17"/>
     <mergeCell ref="J15:J17"/>
@@ -1450,27 +1450,27 @@
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E18" r:id="rId1" display="https://sinta.kemdikbud.go.id/journals/profile/6584" xr:uid="{02F79076-1FD1-4652-BF4F-E5F5609A6461}"/>

</xml_diff>

<commit_message>
Update Black Box Excel
</commit_message>
<xml_diff>
--- a/Rangkuman Jurnal.xlsx
+++ b/Rangkuman Jurnal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCC0C62-A7B7-46E2-9A3A-C5AE33C64587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C488DAB2-D170-4603-8B45-173E3C701F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,8 +477,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -489,8 +489,8 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:E30"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +818,7 @@
       <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -840,7 +840,7 @@
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -976,7 +976,7 @@
       <c r="E10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="18">
         <v>3</v>
       </c>
       <c r="G10" s="17">
@@ -994,7 +994,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="17"/>
       <c r="H11" s="16"/>
     </row>
@@ -1006,7 +1006,7 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="17"/>
       <c r="H12" s="16"/>
     </row>
@@ -1111,22 +1111,22 @@
       <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="14">
         <v>4</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="14">
         <v>2023</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1135,24 +1135,24 @@
       <c r="B19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
@@ -1161,22 +1161,22 @@
       <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="14">
         <v>5</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="14">
         <v>2024</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1185,12 +1185,12 @@
       <c r="B22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
@@ -1446,27 +1446,27 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="I15:I17"/>
     <mergeCell ref="J15:J17"/>
@@ -1483,27 +1483,27 @@
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E18" r:id="rId1" display="https://sinta.kemdikbud.go.id/journals/profile/6584" xr:uid="{02F79076-1FD1-4652-BF4F-E5F5609A6461}"/>

</xml_diff>